<commit_message>
Minden benne van ami kell
</commit_message>
<xml_diff>
--- a/ellenfelek.xlsx
+++ b/ellenfelek.xlsx
@@ -1,25 +1,162 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
     <sheet name="Munka2" sheetId="2" r:id="rId2"/>
     <sheet name="Munka3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+  <si>
+    <t>Név</t>
+  </si>
+  <si>
+    <t>Támadási képesség</t>
+  </si>
+  <si>
+    <t>Védettségi szint</t>
+  </si>
+  <si>
+    <t>Életerő</t>
+  </si>
+  <si>
+    <t>Sikeres támadás esetén életveszteség</t>
+  </si>
+  <si>
+    <t>Megjegyzés</t>
+  </si>
+  <si>
+    <t>Kőszobor</t>
+  </si>
+  <si>
+    <t>2-12(2d6)</t>
+  </si>
+  <si>
+    <t>Lassú, ezért az első csapás a tied</t>
+  </si>
+  <si>
+    <t>Kecskepásztor</t>
+  </si>
+  <si>
+    <t>1-6()</t>
+  </si>
+  <si>
+    <t>Farkasember</t>
+  </si>
+  <si>
+    <t>4-9(d6+3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sámán </t>
+  </si>
+  <si>
+    <t>Kapuőrző Démon</t>
+  </si>
+  <si>
+    <t>5-10(d6+4)</t>
+  </si>
+  <si>
+    <t>Rémkutya</t>
+  </si>
+  <si>
+    <t>Első Kígyó</t>
+  </si>
+  <si>
+    <t>Második Kígyó</t>
+  </si>
+  <si>
+    <t>Mindkét kígyóval egyszerre kell küzdened! 
+Egyiket ütöd másik ellen védekezel.</t>
+  </si>
+  <si>
+    <t>Ajtó</t>
+  </si>
+  <si>
+    <t>1-3(d6/2)</t>
+  </si>
+  <si>
+    <t>Első csapás joga a tied</t>
+  </si>
+  <si>
+    <t>Hószörny</t>
+  </si>
+  <si>
+    <t>3-8(d6+2)</t>
+  </si>
+  <si>
+    <t>Törpe</t>
+  </si>
+  <si>
+    <t>2-7(d6+1)</t>
+  </si>
+  <si>
+    <t>128. Törpe</t>
+  </si>
+  <si>
+    <t>Rabló</t>
+  </si>
+  <si>
+    <t>146. Törpe</t>
+  </si>
+  <si>
+    <t>149. Az alvilág őre</t>
+  </si>
+  <si>
+    <t>151. Jégóriás</t>
+  </si>
+  <si>
+    <t>186. Varázsló</t>
+  </si>
+  <si>
+    <t>Főboss, ha megüt vége a játéknak</t>
+  </si>
+  <si>
+    <t>Harcos nő</t>
+  </si>
+  <si>
+    <t>Minden általad a nőnek okozott sebből mindig vonj le 3 pontot</t>
+  </si>
+  <si>
+    <t>208. Rabló</t>
+  </si>
+  <si>
+    <t>214. Rabló</t>
+  </si>
+  <si>
+    <t>227. Hószörny</t>
+  </si>
+  <si>
+    <t>260. Sivatagi szellem</t>
+  </si>
+  <si>
+    <t>286. Rukh fióka</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -47,8 +184,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -343,12 +491,540 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="18">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="18">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="18">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>80</v>
+      </c>
+      <c r="C6" s="1">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="18">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="24.6" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="18">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="18">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="18">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="18">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="18">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="18">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1">
+        <v>80</v>
+      </c>
+      <c r="C16" s="1">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1">
+        <v>20</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="18">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="18">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="18">
+      <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" ht="18">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="18">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1">
+        <v>18</v>
+      </c>
+      <c r="E23" s="5">
+        <v>4</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="18">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" ht="18">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="18">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="18">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="18">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="18">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" ht="18">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" ht="18">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" ht="18">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" ht="18">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F8:F9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
@@ -360,7 +1036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -373,7 +1049,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>